<commit_message>
Clean up input file and update display
</commit_message>
<xml_diff>
--- a/features/upload-files/test_data.xlsx
+++ b/features/upload-files/test_data.xlsx
@@ -5,17 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyrasis/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyrasis/Desktop/data-dictionary/features/upload-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="2640" windowWidth="28160" windowHeight="11120" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="640" yWindow="2640" windowWidth="28160" windowHeight="11120" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="accession" sheetId="1" r:id="rId1"/>
-    <sheet name="agent_contact" sheetId="2" r:id="rId2"/>
+    <sheet name="agent_contact" sheetId="4" r:id="rId2"/>
     <sheet name="classification_rlshp" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -672,7 +671,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -698,6 +697,22 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -729,8 +744,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -778,7 +797,11 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1788,8 +1811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2422,11 +2445,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G8 G21:G25">
+      <formula1>"The contents of this field are automatically generated by the application.,"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F8 F21:F25">
       <formula1>"Required,Conditional,Not Required"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G8 G21:G25">
-      <formula1>"The contents of this field are automatically generated by the application.,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2788,16 +2811,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>